<commit_message>
Updated Flask app to be memory-friendly and Render-ready
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="212">
   <si>
     <t>VoterID</t>
   </si>
@@ -406,10 +406,13 @@
     <t>सूर्य राम</t>
   </si>
   <si>
+    <t>ः: सहदेव राम</t>
+  </si>
+  <si>
     <t>बल्देव राम</t>
   </si>
   <si>
-    <t>सोमी खतवे</t>
+    <t>ः: सोमी खतवे</t>
   </si>
   <si>
     <t>सूर्य ना राम</t>
@@ -469,7 +472,7 @@
     <t>आलम अंसारी</t>
   </si>
   <si>
-    <t>चन्द्रदेव मंडल</t>
+    <t>ः: चन्द्रदेव मंडल</t>
   </si>
   <si>
     <t>परशुराम यादव</t>
@@ -1039,7 +1042,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="F2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1053,13 +1056,13 @@
         <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1073,13 +1076,13 @@
         <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1093,13 +1096,13 @@
         <v>125</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1113,13 +1116,13 @@
         <v>126</v>
       </c>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1133,13 +1136,13 @@
         <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1153,13 +1156,13 @@
         <v>127</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1173,13 +1176,13 @@
         <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1193,13 +1196,13 @@
         <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F10" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1213,13 +1216,13 @@
         <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1233,13 +1236,13 @@
         <v>128</v>
       </c>
       <c r="D12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E12" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1253,13 +1256,13 @@
         <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F13" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1270,16 +1273,16 @@
         <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E14" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1293,13 +1296,13 @@
         <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F15" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1313,13 +1316,13 @@
         <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E16" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F16" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1330,16 +1333,16 @@
         <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1350,16 +1353,16 @@
         <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1373,13 +1376,13 @@
         <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1390,16 +1393,16 @@
         <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E20" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F20" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1410,16 +1413,16 @@
         <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E21" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F21" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1433,13 +1436,13 @@
         <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1453,13 +1456,13 @@
         <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E23" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1473,13 +1476,13 @@
         <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E24" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1490,16 +1493,16 @@
         <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E25" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F25" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1510,16 +1513,16 @@
         <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D26" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F26" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1530,16 +1533,16 @@
         <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E27" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F27" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1553,13 +1556,13 @@
         <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E28" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F28" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1573,13 +1576,13 @@
         <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E29" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1590,16 +1593,16 @@
         <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E30" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F30" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1610,16 +1613,16 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D31" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E31" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F31" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1630,16 +1633,16 @@
         <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D32" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E32" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F32" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1650,16 +1653,16 @@
         <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E33" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F33" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1670,16 +1673,16 @@
         <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E34" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F34" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1690,16 +1693,16 @@
         <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D35" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E35" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F35" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1713,13 +1716,13 @@
         <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E36" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F36" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1730,16 +1733,16 @@
         <v>99</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E37" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F37" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1750,16 +1753,16 @@
         <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D38" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E38" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F38" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1770,16 +1773,16 @@
         <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D39" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E39" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F39" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1790,16 +1793,16 @@
         <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D40" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E40" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F40" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1810,16 +1813,16 @@
         <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D41" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F41" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1830,16 +1833,16 @@
         <v>104</v>
       </c>
       <c r="C42" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D42" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E42" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F42" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1853,13 +1856,13 @@
         <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E43" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F43" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1870,16 +1873,16 @@
         <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E44" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F44" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1890,16 +1893,16 @@
         <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D45" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E45" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F45" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1910,16 +1913,16 @@
         <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D46" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E46" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F46" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1930,16 +1933,16 @@
         <v>109</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E47" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F47" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1950,16 +1953,16 @@
         <v>110</v>
       </c>
       <c r="C48" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D48" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E48" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F48" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1970,16 +1973,16 @@
         <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E49" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F49" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1990,16 +1993,16 @@
         <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D50" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E50" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F50" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2013,13 +2016,13 @@
         <v>112</v>
       </c>
       <c r="D51" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E51" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F51" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2030,16 +2033,16 @@
         <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E52" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F52" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2050,16 +2053,16 @@
         <v>115</v>
       </c>
       <c r="C53" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D53" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E53" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F53" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2070,16 +2073,16 @@
         <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D54" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E54" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F54" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2090,16 +2093,16 @@
         <v>117</v>
       </c>
       <c r="C55" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D55" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E55" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F55" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2110,16 +2113,16 @@
         <v>118</v>
       </c>
       <c r="C56" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D56" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E56" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F56" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2130,16 +2133,16 @@
         <v>99</v>
       </c>
       <c r="C57" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D57" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E57" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F57" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2150,16 +2153,16 @@
         <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D58" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E58" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F58" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2170,16 +2173,16 @@
         <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D59" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E59" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F59" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2190,16 +2193,16 @@
         <v>121</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D60" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E60" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F60" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2210,16 +2213,16 @@
         <v>122</v>
       </c>
       <c r="C61" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D61" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E61" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F61" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2230,16 +2233,16 @@
         <v>116</v>
       </c>
       <c r="C62" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D62" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E62" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F62" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated memory-friendly PDF processing code
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="211">
   <si>
     <t>VoterID</t>
   </si>
@@ -406,9 +406,6 @@
     <t>सूर्य राम</t>
   </si>
   <si>
-    <t>ः: सहदेव राम</t>
-  </si>
-  <si>
     <t>बल्देव राम</t>
   </si>
   <si>
@@ -472,7 +469,7 @@
     <t>आलम अंसारी</t>
   </si>
   <si>
-    <t>ः: चन्द्रदेव मंडल</t>
+    <t>चन्द्रदेव मंडल</t>
   </si>
   <si>
     <t>परशुराम यादव</t>
@@ -1042,7 +1039,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="F2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1056,13 +1053,13 @@
         <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1076,13 +1073,13 @@
         <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1096,13 +1093,13 @@
         <v>125</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1116,13 +1113,13 @@
         <v>126</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1136,13 +1133,13 @@
         <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1156,13 +1153,13 @@
         <v>127</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1176,13 +1173,13 @@
         <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1196,13 +1193,13 @@
         <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1216,13 +1213,13 @@
         <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1236,13 +1233,13 @@
         <v>128</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1256,13 +1253,13 @@
         <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1273,16 +1270,16 @@
         <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1296,13 +1293,13 @@
         <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1316,13 +1313,13 @@
         <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1333,16 +1330,16 @@
         <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1353,16 +1350,16 @@
         <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1376,13 +1373,13 @@
         <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1393,16 +1390,16 @@
         <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1413,16 +1410,16 @@
         <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1436,13 +1433,13 @@
         <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1456,13 +1453,13 @@
         <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1476,13 +1473,13 @@
         <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1493,16 +1490,16 @@
         <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1513,16 +1510,16 @@
         <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1533,16 +1530,16 @@
         <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1556,13 +1553,13 @@
         <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1576,13 +1573,13 @@
         <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1593,16 +1590,16 @@
         <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1613,16 +1610,16 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1633,16 +1630,16 @@
         <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1653,16 +1650,16 @@
         <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1673,16 +1670,16 @@
         <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1693,16 +1690,16 @@
         <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1716,13 +1713,13 @@
         <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1733,16 +1730,16 @@
         <v>99</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1753,16 +1750,16 @@
         <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1773,16 +1770,16 @@
         <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1793,16 +1790,16 @@
         <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F40" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1813,16 +1810,16 @@
         <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1833,16 +1830,16 @@
         <v>104</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1856,13 +1853,13 @@
         <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1873,16 +1870,16 @@
         <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E44" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1893,16 +1890,16 @@
         <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1913,16 +1910,16 @@
         <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1933,16 +1930,16 @@
         <v>109</v>
       </c>
       <c r="C47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1953,16 +1950,16 @@
         <v>110</v>
       </c>
       <c r="C48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1973,16 +1970,16 @@
         <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E49" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F49" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1993,16 +1990,16 @@
         <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2016,13 +2013,13 @@
         <v>112</v>
       </c>
       <c r="D51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E51" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F51" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2033,16 +2030,16 @@
         <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F52" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2053,16 +2050,16 @@
         <v>115</v>
       </c>
       <c r="C53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D53" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E53" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F53" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2073,16 +2070,16 @@
         <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D54" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E54" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2093,16 +2090,16 @@
         <v>117</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2113,16 +2110,16 @@
         <v>118</v>
       </c>
       <c r="C56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F56" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2133,16 +2130,16 @@
         <v>99</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D57" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E57" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F57" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2153,16 +2150,16 @@
         <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D58" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E58" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2173,16 +2170,16 @@
         <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D59" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F59" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2193,16 +2190,16 @@
         <v>121</v>
       </c>
       <c r="C60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2213,16 +2210,16 @@
         <v>122</v>
       </c>
       <c r="C61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D61" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2233,16 +2230,16 @@
         <v>116</v>
       </c>
       <c r="C62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D62" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F62" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>